<commit_message>
moved to week 6
</commit_message>
<xml_diff>
--- a/result_list_round_2.xlsx
+++ b/result_list_round_2.xlsx
@@ -463,37 +463,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mo' Money Mo Bamba (2)</t>
+          <t>Mo' Money Mo Bamba (7)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Team Becks (7)</t>
+          <t>Team Becks (3)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Mo' Money Mo Bamba</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Team Becks</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Mo' Money Mo Bamba</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Gaza Gunners (4)</t>
+          <t>Gaza Gunners (2)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Los Angeles Ballerz (6)</t>
+          <t>Los Angeles Ballerz (8)</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -513,12 +513,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Chi Cargo Pants (5)</t>
+          <t>Chi Cargo Pants (6)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GIDDEY UPS - MAILMAN 2.0 (6)</t>
+          <t>GIDDEY UPS - MAILMAN 2.0 (5)</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -526,24 +526,24 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Chi Cargo Pants</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>GIDDEY UPS - MAILMAN 2.0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Chi Cargo Pants</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Harrison the league (8)</t>
+          <t>Harrison the league (2)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Memphis 12 Guage (2)</t>
+          <t>Memphis 12 Guage (8)</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -551,28 +551,28 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Memphis 12 Guage</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Harrison the league</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Memphis 12 Guage</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Giddey Up Chumps (4)</t>
+          <t>Giddey Up Chumps (2)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wham Bam Thankyou Ma’am (5)</t>
+          <t>Wham Bam Thankyou Ma’am (9)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -588,20 +588,20 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Phoenix Gray Hammers (3)</t>
+          <t>Phoenix Gray Hammers (4)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Team Wallace (7)</t>
+          <t>Team Winchester (7)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Team Wallace</t>
+          <t>Team Winchester</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -613,41 +613,41 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Brooklyn 99 (4)</t>
+          <t>Brooklyn 99 (8)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Brooks, Crooks and Sooks (6)</t>
+          <t>Brooks, Crooks and Sooks (3)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Brooklyn 99</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Brooks, Crooks and Sooks</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Brooklyn 99</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Keyonte George Costanza (6)</t>
+          <t>Keyonte George Costanza (8)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Landsdale Smith (3)</t>
+          <t>Landsdale Smith (2)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -663,12 +663,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Under my Clint Capela (5)</t>
+          <t>Under my Clint Capela (3)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Who what where when Kawhi (6)</t>
+          <t>Who what where when Kawhi (7)</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -688,12 +688,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ol' Dirty Baskets (6)</t>
+          <t>Ol' Dirty Baskets (5)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The David Cahill's (5)</t>
+          <t>The Flaming Galahs (6)</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -701,24 +701,24 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>The Flaming Galahs</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Ol' Dirty Baskets</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>The David Cahill's</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dallas Double D's (3)</t>
+          <t>Dallas Double D's (1)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Funghi Curry (7)</t>
+          <t>Funghi Curry (9)</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -738,16 +738,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Matisse Fly Bulls (4)</t>
+          <t>Matisse Fly Bulls (3)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TankCity Unicorns (6)</t>
+          <t>TankCity Unicorns (8)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -763,12 +763,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OKC-OOPS (7)</t>
+          <t>OKC-OOPS (9)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>VICTOR-IOUS (3)</t>
+          <t>VICTOR-IOUS (1)</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -788,12 +788,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Team irwin (8)</t>
+          <t>Team irwin (6)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tennant Creek Big Horses (2)</t>
+          <t>The A**L Embiids (5)</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -806,19 +806,19 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Tennant Creek Big Horses</t>
+          <t>The A**L Embiids</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Edward St Easybeats (5)</t>
+          <t>Edward St Easybeats (6)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Josh Kiddey (6)</t>
+          <t>Josh Kiddey (5)</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -826,24 +826,24 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>Edward St Easybeats</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>Josh Kiddey</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Edward St Easybeats</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Flex n Affect (7)</t>
+          <t>Flex n Affect (6)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Moon Shooters (3)</t>
+          <t>Moon Shooters (4)</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -863,87 +863,87 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jimmy Brings (6)</t>
+          <t>Jimmy Brings (5)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The Plasticman (4)</t>
+          <t>The Sengunies (6)</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>The Sengunies</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>Jimmy Brings</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>The Plasticman</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Daryl's Discount Dimes (6)</t>
+          <t>Daryl's Discount Dimes (3)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Slovenia. Beer. Dallas (5)</t>
+          <t>Slovenia. Beer. Dallas (6)</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>Slovenia. Beer. Dallas</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>Daryl's Discount Dimes</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Slovenia. Beer. Dallas</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Adelaide Shed Shots (3)</t>
+          <t>Adelaide Shed Shots (6)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Minnesota Lumberjacks (7)</t>
+          <t>Minnesota Lumberjacks (3)</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>Adelaide Shed Shots</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>Minnesota Lumberjacks</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Adelaide Shed Shots</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ANUS BLEACHING SEA LIONS (7)</t>
+          <t>ANUS BLEACHING SEA LIONS (6)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>New York NateThrobinsons (3)</t>
+          <t>New York NateThrobinsons (5)</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -963,41 +963,41 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Team Blah (4)</t>
+          <t>Team Blah (6)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The Chet Code (6)</t>
+          <t>The David Cahill's (5)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>The Chet Code</t>
+          <t>Team Blah</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Team Blah</t>
+          <t>The David Cahill's</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Luka Warm (6)</t>
+          <t>Luka Warm (9)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Team Cumming (4)</t>
+          <t>Team Cumming (2)</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1013,62 +1013,62 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Balls Deep (6)</t>
+          <t>Balls Deep (2)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Team James (3)</t>
+          <t>Team James (8)</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>Team James</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>Balls Deep</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Team James</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Browntown (3)</t>
+          <t>Browntown (7)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Scottie Pippings (6)</t>
+          <t>Scottie Pippings (3)</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>Browntown</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>Scottie Pippings</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Browntown</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Gladysisahoe Dazz (7)</t>
+          <t>Gladysisahoe Dazz (6)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Lucky Punters (3)</t>
+          <t>Lucky Punters (5)</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1088,16 +1088,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bronsexual Lebrolites (5)</t>
+          <t>Bronsexual Lebrolites (8)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Team Thomas (4)</t>
+          <t>Team Wallace (3)</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1106,19 +1106,19 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Team Thomas</t>
+          <t>Team Wallace</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Atlanta Waivers (7)</t>
+          <t>Atlanta Waivers (8)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Insert Team Name Here (3)</t>
+          <t>Insert Team Name Here (2)</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1138,16 +1138,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Taiwan Troopers (4)</t>
+          <t>Taiwan Troopers (1)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>War Grimes in Garza (6)</t>
+          <t>War Grimes in Garza (10)</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1163,12 +1163,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Allen In Shorts (4)</t>
+          <t>Allen In Shorts (1)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jaylen CAN go left! (6)</t>
+          <t>Jaylen CAN go left! (9)</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1188,37 +1188,37 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Boswell Pioneers (2)</t>
+          <t>Boswell Pioneers (6)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Mile High Mutombo's (8)</t>
+          <t>Mile High Mutombo's (5)</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>Boswell Pioneers</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>Mile High Mutombo's</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Boswell Pioneers</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Boots Manuva (8)</t>
+          <t>Boots Manuva (2)</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Hispanic Deepers (2)</t>
+          <t>Hispanic Deepers (8)</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
+          <t>Hispanic Deepers</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>Boots Manuva</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Hispanic Deepers</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Little Buff Boys (6)</t>
+          <t>Little Buff Boys (1)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Miami Heat Checks (5)</t>
+          <t>Miami Heat Checks (9)</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1251,24 +1251,24 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>Miami Heat Checks</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>Little Buff Boys</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Miami Heat Checks</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Donnys Beans (6)</t>
+          <t>Donnys Beans (2)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LIL UZI YURT (5)</t>
+          <t>LIL UZI YURT (8)</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1276,24 +1276,24 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
+          <t>LIL UZI YURT</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
           <t>Donnys Beans</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>LIL UZI YURT</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GOLD COAST GREMLINS (7)</t>
+          <t>GOLD COAST GREMLINS (2)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Quit Javing me turky (3)</t>
+          <t>Quit Javing me turky (8)</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1301,12 +1301,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>Quit Javing me turky</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>GOLD COAST GREMLINS</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Quit Javing me turky</t>
         </is>
       </c>
     </row>
@@ -1363,12 +1363,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BigZ Spurs (6)</t>
+          <t>BigZ Spurs (7)</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Team Hewish (5)</t>
+          <t>Team Hewish (4)</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1413,12 +1413,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Moves Like Agger (6)</t>
+          <t>Moves Like Agger (1)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The Blue Mountain Goats (4)</t>
+          <t>The Book of Irving (9)</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1426,28 +1426,28 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>The Book of Irving</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>Moves Like Agger</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>The Blue Mountain Goats</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SavedByTheKelle (7)</t>
+          <t>SavedByTheKelle (6)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Zions Illegitimate Child (3)</t>
+          <t>Zions Illegitimate Child (5)</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1468,15 +1468,15 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>The Great Hali (5)</t>
+          <t>The Hairy Skips (7)</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>The Great Hali</t>
+          <t>The Hairy Skips</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1488,12 +1488,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ROUdiamondGH (7)</t>
+          <t>ROUdiamondGH (6)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Victor Oladeepthr*ats (3)</t>
+          <t>Victor Oladeepthr*ats (4)</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1513,12 +1513,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Margaret River Wyld Stallyns (3)</t>
+          <t>Margaret River Wyld Stallyns (4)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OG Wan Unobi (8)</t>
+          <t>OG Wan Unobi (7)</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1538,12 +1538,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>BIG BULLS (7)</t>
+          <t>BIG BULLS (6)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Team Damon (4)</t>
+          <t>Team Damon (5)</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1563,12 +1563,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Bank Town Squids (7)</t>
+          <t>Bank Town Squids (6)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>You Don't Mess with the Ant-Man (3)</t>
+          <t>You Don't Mess with the Ant-Man (4)</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1588,12 +1588,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>The Hairy Skips (6)</t>
+          <t>The IBINATORS (7)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Uncle Ben (4)</t>
+          <t>Uncle Ben (3)</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>The Hairy Skips</t>
+          <t>The IBINATORS</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1613,7 +1613,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ChixnGrog (6)</t>
+          <t>ChixnGrog (5)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1638,20 +1638,20 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>The Book of Irving (9)</t>
+          <t>The Bricks (5)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Weekend at Boogie's (1)</t>
+          <t>Weekend at Boogie's (4)</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>The Book of Irving</t>
+          <t>The Bricks</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1663,7 +1663,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Lukatmenowmum (4)</t>
+          <t>Lukatmenowmum (5)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1713,12 +1713,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ja 'his real name is Clarence' (8)</t>
+          <t>Ja 'his real name is Clarence' (6)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Team luka slo (2)</t>
+          <t>Team luka slo (4)</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1738,12 +1738,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Caruso BaldEagles (3)</t>
+          <t>Caruso BaldEagles (7)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Houston Mob Squad (7)</t>
+          <t>Houston Mob Squad (3)</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1751,12 +1751,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
+          <t>Caruso BaldEagles</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
           <t>Houston Mob Squad</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Caruso BaldEagles</t>
         </is>
       </c>
     </row>
@@ -1768,11 +1768,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Townsville Crocs (8)</t>
+          <t>Townsville Crocs (7)</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1788,16 +1788,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Ben Simmons Construction (4)</t>
+          <t>Ben Simmons Construction (3)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Indiana Monstars (5)</t>
+          <t>Indiana Monstars (7)</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1813,12 +1813,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Joeys Mad Lads (5)</t>
+          <t>Joeys Mad Lads (4)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Red Dragons (6)</t>
+          <t>Red Dragons (7)</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1847,7 +1847,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1863,12 +1863,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Signature Moves (6)</t>
+          <t>Signature Moves (3)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Team Pyke (4)</t>
+          <t>Team Pyke (7)</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1876,28 +1876,28 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
+          <t>Team Pyke</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
           <t>Signature Moves</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>Team Pyke</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Ja Raffe (6)</t>
+          <t>Ja Raffe (5)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Joe Hablo Ingles (5)</t>
+          <t>Joe Hablo Ingles (4)</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1913,12 +1913,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Kobe Beans (4)</t>
+          <t>Kobe Beans (2)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>The Flaming Galahs (7)</t>
+          <t>The Gee Whizzles (9)</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>The Flaming Galahs</t>
+          <t>The Gee Whizzles</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1938,12 +1938,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Dort Stop Believin (7)</t>
+          <t>Dort Stop Believin (10)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Round Mound of Rebound (3)</t>
+          <t>Round Mound of Rebound (0)</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1963,32 +1963,32 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Hard Solo (1)</t>
+          <t>Hard Solo (6)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Valentuna Sandwhich (8)</t>
+          <t>Valentuna Sandwhich (5)</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
+          <t>Hard Solo</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
           <t>Valentuna Sandwhich</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Hard Solo</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Boston Bombers (4)</t>
+          <t>Boston Bombers (5)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2013,12 +2013,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Boomtown Bulls (7)</t>
+          <t>Boomtown Bulls (8)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Shanghai Sharks (3)</t>
+          <t>Shanghai Sharks (2)</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -2038,16 +2038,16 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Boston Ballerz (4)</t>
+          <t>Boston Ballerz (3)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Duncans Donuts (6)</t>
+          <t>Duncans Donuts (8)</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2063,12 +2063,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>James and the Giant Overreach (6)</t>
+          <t>James and the Giant Overreach (4)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Peeattle Poopersonics (4)</t>
+          <t>Peeattle Poopersonics (6)</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -2076,12 +2076,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
+          <t>Peeattle Poopersonics</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
           <t>James and the Giant Overreach</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Peeattle Poopersonics</t>
         </is>
       </c>
     </row>

</xml_diff>